<commit_message>
Wednesday second week push
</commit_message>
<xml_diff>
--- a/data/population_projections_by_race_age_groups_IRF_counties_23_25.xlsx
+++ b/data/population_projections_by_race_age_groups_IRF_counties_23_25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgcar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgcar\Documents\NSS_dda16\Capstone\North_Carolina_Inpatient_Rehab_Hospital_Quality_Measures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E422112C-8D4C-4D6D-81B5-2719E3480970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE85E971-C986-41A1-9865-358375DED367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="26070" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1307,9 +1307,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="28.796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -2933,7 +2936,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -3049,7 +3052,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -3165,7 +3168,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -3281,7 +3284,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3745,7 +3748,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -4093,7 +4096,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -4441,7 +4444,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -4557,7 +4560,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -4673,7 +4676,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -4789,7 +4792,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -4905,7 +4908,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -5021,7 +5024,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -5137,7 +5140,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -5253,7 +5256,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -5369,7 +5372,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>126</v>
       </c>
@@ -5485,7 +5488,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -5601,7 +5604,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -5717,7 +5720,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -5833,7 +5836,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -5949,7 +5952,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>101</v>
       </c>
@@ -6065,7 +6068,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>126</v>
       </c>
@@ -6181,7 +6184,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -6297,7 +6300,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -6413,7 +6416,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -6529,7 +6532,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -6645,7 +6648,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -6761,7 +6764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -6877,7 +6880,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -6993,7 +6996,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -7109,7 +7112,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -7225,7 +7228,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -7341,7 +7344,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>120</v>
       </c>
@@ -7457,7 +7460,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -7573,7 +7576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -7689,7 +7692,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>89</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -7921,7 +7924,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -8037,7 +8040,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -8153,7 +8156,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -8269,7 +8272,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -8385,7 +8388,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>111</v>
       </c>
@@ -8501,7 +8504,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -8617,7 +8620,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -8733,7 +8736,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -8849,7 +8852,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -8965,7 +8968,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -9081,7 +9084,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>111</v>
       </c>
@@ -9197,7 +9200,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>115</v>
       </c>
@@ -9313,7 +9316,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -9429,7 +9432,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>126</v>
       </c>
@@ -9545,7 +9548,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>126</v>
       </c>
@@ -9661,7 +9664,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -9777,7 +9780,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>131</v>
       </c>
@@ -9893,7 +9896,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>115</v>
       </c>
@@ -10009,7 +10012,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -10125,7 +10128,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -10241,7 +10244,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>65</v>
       </c>
@@ -10357,7 +10360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -10473,7 +10476,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -10589,7 +10592,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>105</v>
       </c>
@@ -10705,7 +10708,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -10821,7 +10824,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -10937,7 +10940,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -11053,7 +11056,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>120</v>
       </c>
@@ -11169,7 +11172,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>120</v>
       </c>
@@ -11285,7 +11288,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>65</v>
       </c>
@@ -11401,7 +11404,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>126</v>
       </c>
@@ -11517,7 +11520,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>136</v>
       </c>
@@ -11633,7 +11636,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -11749,7 +11752,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -11865,7 +11868,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -11981,7 +11984,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>126</v>
       </c>
@@ -12097,7 +12100,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>38</v>
       </c>
@@ -12213,7 +12216,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -12329,7 +12332,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -12445,7 +12448,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>136</v>
       </c>
@@ -12561,7 +12564,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>136</v>
       </c>
@@ -12677,7 +12680,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -12793,7 +12796,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>95</v>
       </c>
@@ -12909,7 +12912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>55</v>
       </c>
@@ -13025,7 +13028,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -13141,7 +13144,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -13257,7 +13260,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>78</v>
       </c>
@@ -13373,7 +13376,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>95</v>
       </c>
@@ -13489,7 +13492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -13605,7 +13608,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>120</v>
       </c>
@@ -13721,7 +13724,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -13837,7 +13840,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>55</v>
       </c>
@@ -13953,7 +13956,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -14069,7 +14072,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>95</v>
       </c>
@@ -14185,7 +14188,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>105</v>
       </c>
@@ -14301,7 +14304,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>95</v>
       </c>
@@ -14417,7 +14420,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>71</v>
       </c>
@@ -14533,7 +14536,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>126</v>
       </c>
@@ -14649,7 +14652,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -14765,7 +14768,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>84</v>
       </c>
@@ -14881,7 +14884,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>78</v>
       </c>
@@ -14997,7 +15000,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>111</v>
       </c>
@@ -15113,7 +15116,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>78</v>
       </c>
@@ -15229,7 +15232,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>131</v>
       </c>
@@ -15345,7 +15348,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>101</v>
       </c>
@@ -15461,7 +15464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>105</v>
       </c>
@@ -15577,7 +15580,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>101</v>
       </c>
@@ -15693,7 +15696,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>84</v>
       </c>
@@ -15809,7 +15812,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>131</v>
       </c>
@@ -15925,7 +15928,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>136</v>
       </c>
@@ -16041,7 +16044,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>131</v>
       </c>
@@ -16157,7 +16160,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>111</v>
       </c>
@@ -16273,7 +16276,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>120</v>
       </c>
@@ -16389,7 +16392,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>105</v>
       </c>
@@ -16505,7 +16508,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>65</v>
       </c>
@@ -16621,7 +16624,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>95</v>
       </c>
@@ -16737,7 +16740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>95</v>
       </c>
@@ -16853,7 +16856,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>38</v>
       </c>
@@ -16969,7 +16972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>48</v>
       </c>
@@ -17085,7 +17088,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>84</v>
       </c>
@@ -17201,7 +17204,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>78</v>
       </c>
@@ -17317,7 +17320,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>65</v>
       </c>
@@ -17433,7 +17436,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>38</v>
       </c>
@@ -17549,7 +17552,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>38</v>
       </c>
@@ -17665,7 +17668,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>131</v>
       </c>
@@ -17781,7 +17784,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>131</v>
       </c>
@@ -17897,7 +17900,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>120</v>
       </c>
@@ -18013,7 +18016,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>120</v>
       </c>
@@ -18129,7 +18132,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>101</v>
       </c>
@@ -18245,7 +18248,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>105</v>
       </c>
@@ -18361,7 +18364,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>105</v>
       </c>
@@ -18477,7 +18480,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>115</v>
       </c>
@@ -18593,7 +18596,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>84</v>
       </c>
@@ -18709,7 +18712,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>95</v>
       </c>
@@ -18825,7 +18828,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>105</v>
       </c>
@@ -18941,7 +18944,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>115</v>
       </c>
@@ -19057,7 +19060,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>101</v>
       </c>
@@ -19173,7 +19176,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>38</v>
       </c>
@@ -19289,7 +19292,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>105</v>
       </c>
@@ -19405,7 +19408,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>65</v>
       </c>
@@ -19521,7 +19524,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>111</v>
       </c>
@@ -19637,7 +19640,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>95</v>
       </c>
@@ -19753,7 +19756,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>136</v>
       </c>
@@ -19869,7 +19872,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>105</v>
       </c>
@@ -19985,7 +19988,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>78</v>
       </c>
@@ -20101,7 +20104,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>111</v>
       </c>
@@ -20217,7 +20220,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>120</v>
       </c>
@@ -20333,7 +20336,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>136</v>
       </c>
@@ -20449,7 +20452,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>95</v>
       </c>
@@ -20565,7 +20568,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>126</v>
       </c>
@@ -20681,7 +20684,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>120</v>
       </c>
@@ -20797,7 +20800,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>111</v>
       </c>
@@ -20913,7 +20916,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>89</v>
       </c>
@@ -21029,7 +21032,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>89</v>
       </c>
@@ -21145,7 +21148,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>84</v>
       </c>
@@ -21261,7 +21264,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>55</v>
       </c>
@@ -21377,7 +21380,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>38</v>
       </c>
@@ -21493,7 +21496,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>131</v>
       </c>
@@ -21609,7 +21612,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>55</v>
       </c>
@@ -21725,7 +21728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>55</v>
       </c>
@@ -21841,7 +21844,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>131</v>
       </c>
@@ -21957,7 +21960,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>55</v>
       </c>
@@ -22073,7 +22076,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>89</v>
       </c>
@@ -22189,7 +22192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>126</v>
       </c>
@@ -22305,7 +22308,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>115</v>
       </c>
@@ -22421,7 +22424,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>115</v>
       </c>
@@ -22537,7 +22540,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>84</v>
       </c>
@@ -22653,7 +22656,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>101</v>
       </c>
@@ -22769,7 +22772,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>136</v>
       </c>
@@ -22885,7 +22888,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>131</v>
       </c>
@@ -23001,7 +23004,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>38</v>
       </c>
@@ -23117,7 +23120,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>84</v>
       </c>
@@ -23233,7 +23236,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>126</v>
       </c>
@@ -23349,7 +23352,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>111</v>
       </c>
@@ -23465,7 +23468,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>95</v>
       </c>
@@ -23581,7 +23584,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>115</v>
       </c>
@@ -23697,7 +23700,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>65</v>
       </c>
@@ -23813,7 +23816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>78</v>
       </c>
@@ -23929,7 +23932,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>89</v>
       </c>
@@ -24045,7 +24048,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>105</v>
       </c>
@@ -24161,7 +24164,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>136</v>
       </c>
@@ -24277,7 +24280,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="199" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>38</v>
       </c>
@@ -24393,7 +24396,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="200" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -24509,7 +24512,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="201" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>55</v>
       </c>
@@ -24625,7 +24628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="202" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>136</v>
       </c>
@@ -24741,7 +24744,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="203" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>136</v>
       </c>
@@ -24857,7 +24860,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="204" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>101</v>
       </c>
@@ -24973,7 +24976,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="205" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>78</v>
       </c>
@@ -25089,7 +25092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="206" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>95</v>
       </c>
@@ -25205,7 +25208,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="207" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>126</v>
       </c>
@@ -25321,7 +25324,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="208" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>120</v>
       </c>
@@ -25437,7 +25440,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="209" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>120</v>
       </c>
@@ -25553,7 +25556,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="210" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>136</v>
       </c>
@@ -25669,7 +25672,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="211" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>38</v>
       </c>
@@ -25785,7 +25788,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="212" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>71</v>
       </c>
@@ -25901,7 +25904,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="213" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>65</v>
       </c>
@@ -26017,7 +26020,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="214" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>38</v>
       </c>
@@ -26133,7 +26136,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="215" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>84</v>
       </c>
@@ -26249,7 +26252,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="216" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>111</v>
       </c>
@@ -26365,7 +26368,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="217" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>131</v>
       </c>
@@ -26481,7 +26484,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="218" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>71</v>
       </c>
@@ -26597,7 +26600,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="219" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>111</v>
       </c>
@@ -26713,7 +26716,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="220" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>95</v>
       </c>
@@ -26829,7 +26832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="221" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>115</v>
       </c>
@@ -26945,7 +26948,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="222" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>131</v>
       </c>
@@ -27061,7 +27064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="223" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>126</v>
       </c>
@@ -27177,7 +27180,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="224" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>105</v>
       </c>
@@ -27293,7 +27296,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="225" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>48</v>
       </c>
@@ -27409,7 +27412,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="226" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>105</v>
       </c>
@@ -27525,7 +27528,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="227" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>38</v>
       </c>
@@ -27641,7 +27644,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="228" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>115</v>
       </c>
@@ -27757,7 +27760,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="229" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>95</v>
       </c>
@@ -27873,7 +27876,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="230" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>48</v>
       </c>
@@ -27989,7 +27992,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="231" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>65</v>
       </c>
@@ -28105,7 +28108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="232" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>71</v>
       </c>
@@ -28221,7 +28224,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="233" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>84</v>
       </c>
@@ -28337,7 +28340,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="234" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>55</v>
       </c>
@@ -28453,7 +28456,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="235" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>71</v>
       </c>
@@ -28569,7 +28572,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="236" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>101</v>
       </c>
@@ -28685,7 +28688,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="237" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>131</v>
       </c>
@@ -28801,7 +28804,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="238" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>65</v>
       </c>
@@ -28917,7 +28920,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="239" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>71</v>
       </c>
@@ -29033,7 +29036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="240" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>101</v>
       </c>
@@ -29149,7 +29152,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="241" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>115</v>
       </c>
@@ -29265,7 +29268,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="242" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>89</v>
       </c>
@@ -29381,7 +29384,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="243" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>136</v>
       </c>
@@ -29497,7 +29500,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="244" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>126</v>
       </c>
@@ -29613,7 +29616,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="245" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>111</v>
       </c>
@@ -29729,7 +29732,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="246" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>89</v>
       </c>
@@ -29845,7 +29848,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="247" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>89</v>
       </c>
@@ -29961,7 +29964,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="248" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>131</v>
       </c>
@@ -30077,7 +30080,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="249" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>136</v>
       </c>
@@ -30193,7 +30196,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="250" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>136</v>
       </c>
@@ -30309,7 +30312,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="251" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>115</v>
       </c>
@@ -30425,7 +30428,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="252" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>136</v>
       </c>
@@ -30541,7 +30544,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="253" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>101</v>
       </c>

</xml_diff>